<commit_message>
Completed Relevance Judment on 25 Querys. See QUery Ranking.xlsx File for summary.
</commit_message>
<xml_diff>
--- a/Query Ranking.xlsx
+++ b/Query Ranking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MonyPC\Desktop\CS410\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DBE750-6EF9-4A2C-B55B-3EA7404F1C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE253BB-13DC-49A6-9E6A-2850A73A2B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16260" xr2:uid="{0F9C3B2E-1E48-4CEB-81D7-8A78688B1683}"/>
+    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{0F9C3B2E-1E48-4CEB-81D7-8A78688B1683}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="185">
   <si>
     <t>Revelant ?</t>
   </si>
@@ -389,6 +389,204 @@
   </si>
   <si>
     <t>2012 elections in India</t>
+  </si>
+  <si>
+    <t>Canine coronavirus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coronavirus  </t>
+  </si>
+  <si>
+    <t>Evoked potential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Economic Stimulus Act of 2008 </t>
+  </si>
+  <si>
+    <t>Exposure and response prevention</t>
+  </si>
+  <si>
+    <t>Arab League–Iran relations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timeline of the nuclear program of Iran </t>
+  </si>
+  <si>
+    <t>Iran Air</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dalit Panther</t>
+  </si>
+  <si>
+    <t>Black Panther Party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parasitism  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parasitology  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brood parasite </t>
+  </si>
+  <si>
+    <t>Cultural impact of Wonder Woman</t>
+  </si>
+  <si>
+    <t>Wonder Girl</t>
+  </si>
+  <si>
+    <t>Marvel Entertainment</t>
+  </si>
+  <si>
+    <t>Marvel Family</t>
+  </si>
+  <si>
+    <t>Marvel Animation</t>
+  </si>
+  <si>
+    <t>Gotham City Sirens</t>
+  </si>
+  <si>
+    <t>Gotham Girls</t>
+  </si>
+  <si>
+    <t>Harley Quinn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> History of the Miami Heat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bulls–Heat rivalry </t>
+  </si>
+  <si>
+    <t>Heat–Knicks rivalry</t>
+  </si>
+  <si>
+    <t>2013–14 Dallas Stars season</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2012–13 Dallas Stars season </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matt Dallas  Matthew Joseph </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arrowhead Stadium </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  2003 Kansas City Chiefs season</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2008 Kansas City Chiefs season</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bell state </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anton Zeilinger </t>
+  </si>
+  <si>
+    <t>Quantum entanglement</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Influenza pandemic</t>
+  </si>
+  <si>
+    <t>Human mortality from H5N1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pandemic Studios  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Asymptomatic carrier </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Systemic primary carnitine deficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Asymptomatic</t>
+  </si>
+  <si>
+    <t>Christiaan Van Vuuren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quarantine  </t>
+  </si>
+  <si>
+    <t>Australian Quarantine and Inspection Service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Blitar  Blitar is a city in East Java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Five Precepts </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Simon Spurrier  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> United States federal government shutdown of 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Willie Horton  William R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Furlough  </t>
+  </si>
+  <si>
+    <t>The Chitling test  Originally named the Dove Counterbalance General Intelligence Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juneteenth  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ralph Ellison </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catherine M. Russell </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Joe Biden  Joseph Robinette "Joe" Biden</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jill Biden </t>
+  </si>
+  <si>
+    <t>The Perfect Mate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">California Attorney General </t>
+  </si>
+  <si>
+    <t>Kamala Nehru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayor of London </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Boris Johnson  Alexander</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marina Wheeler</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Richard Mourdock </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Malta national football team </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gianluca Bezzina</t>
+  </si>
+  <si>
+    <t>Republican Governors Association</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Daniel L. Doctoroff </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rabbit Fur Coat</t>
   </si>
 </sst>
 </file>
@@ -435,7 +633,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,13 +654,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -866,7 +1070,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -961,61 +1165,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1332,10 +1539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A6696D-5153-405F-8D08-2635F4023E1D}">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1344,12 +1551,12 @@
     <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="53" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" style="53" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="53" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="45" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="79.140625" style="45" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
@@ -1372,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1395,24 +1602,24 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="20"/>
       <c r="C3" s="36"/>
       <c r="D3" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="41">
+      <c r="E3" s="40">
         <v>55578</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="G3" s="56" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="21"/>
       <c r="C4" s="36"/>
@@ -1425,11 +1632,11 @@
       <c r="F4" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G4" s="55" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="G4" s="53" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>2</v>
       </c>
@@ -1440,51 +1647,51 @@
       <c r="D5" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="44">
+      <c r="E5" s="41">
         <v>1359710</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="41" t="s">
         <v>116</v>
       </c>
       <c r="G5" s="54" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="23"/>
       <c r="C6" s="36"/>
       <c r="D6" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="42">
         <v>1442015</v>
       </c>
-      <c r="F6" s="46" t="s">
+      <c r="F6" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="G6" s="57" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="51" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17"/>
       <c r="B7" s="24"/>
       <c r="C7" s="36"/>
       <c r="D7" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="48">
+      <c r="E7" s="43">
         <v>31757741</v>
       </c>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="G7" s="58" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="G7" s="52" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>3</v>
       </c>
@@ -1495,33 +1702,51 @@
       <c r="D8" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="50"/>
-    </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="E8" s="57">
+        <v>201983</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="55" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="20"/>
       <c r="C9" s="36"/>
       <c r="D9" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="42"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="40">
+        <v>3838061</v>
+      </c>
+      <c r="F9" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" s="51" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="21"/>
       <c r="C10" s="36"/>
       <c r="D10" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="43"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="E10" s="56">
+        <v>201983</v>
+      </c>
+      <c r="F10" s="58" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="53" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>4</v>
       </c>
@@ -1532,33 +1757,51 @@
       <c r="D11" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="45"/>
-    </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="E11" s="41">
+        <v>15678104</v>
+      </c>
+      <c r="F11" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="54" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="23"/>
       <c r="C12" s="36"/>
       <c r="D12" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="47"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="42">
+        <v>176315</v>
+      </c>
+      <c r="F12" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="24"/>
       <c r="C13" s="36"/>
       <c r="D13" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="49"/>
-    </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="E13" s="43">
+        <v>1471006</v>
+      </c>
+      <c r="F13" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" s="48" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>5</v>
       </c>
@@ -1569,31 +1812,50 @@
       <c r="D14" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="50"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="E14" s="3">
+        <v>168635</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G14" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="I14" s="49"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="20"/>
       <c r="C15" s="36"/>
       <c r="D15" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="42"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="40">
+        <v>10340960</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" s="51" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="26"/>
       <c r="C16" s="37"/>
       <c r="D16" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="52"/>
+      <c r="E16" s="44">
+        <v>4684993</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="G16" s="52" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
@@ -1608,9 +1870,15 @@
       <c r="D17" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="45"/>
+      <c r="E17" s="41">
+        <v>25740371</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" s="47" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
@@ -1619,9 +1887,15 @@
       <c r="D18" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="47"/>
+      <c r="E18" s="42">
+        <v>1083841</v>
+      </c>
+      <c r="F18" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="51" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17"/>
@@ -1630,9 +1904,15 @@
       <c r="D19" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="49"/>
+      <c r="E19" s="43">
+        <v>23278339</v>
+      </c>
+      <c r="F19" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="G19" s="48" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
@@ -1645,9 +1925,15 @@
       <c r="D20" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="50"/>
+      <c r="E20" s="3">
+        <v>43937</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G20" s="55" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
@@ -1656,9 +1942,15 @@
       <c r="D21" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="42"/>
+      <c r="E21" s="40">
+        <v>608181</v>
+      </c>
+      <c r="F21" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="G21" s="51" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
@@ -1667,9 +1959,15 @@
       <c r="D22" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="43"/>
+      <c r="E22" s="2">
+        <v>383854</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G22" s="53" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
@@ -1682,9 +1980,15 @@
       <c r="D23" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="45"/>
+      <c r="E23" s="41">
+        <v>861098</v>
+      </c>
+      <c r="F23" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="G23" s="47" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
@@ -1693,9 +1997,15 @@
       <c r="D24" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="47"/>
+      <c r="E24" s="42">
+        <v>5451425</v>
+      </c>
+      <c r="F24" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" s="51" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="17"/>
@@ -1704,9 +2014,15 @@
       <c r="D25" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="49"/>
+      <c r="E25" s="43">
+        <v>111582</v>
+      </c>
+      <c r="F25" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="52" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
@@ -1719,9 +2035,15 @@
       <c r="D26" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="50"/>
+      <c r="E26" s="3">
+        <v>5727147</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G26" s="55" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
@@ -1730,9 +2052,15 @@
       <c r="D27" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="42"/>
+      <c r="E27" s="40">
+        <v>5027882</v>
+      </c>
+      <c r="F27" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="G27" s="51" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
@@ -1741,9 +2069,15 @@
       <c r="D28" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="43"/>
+      <c r="E28" s="2">
+        <v>1160627</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G28" s="53" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
@@ -1756,9 +2090,15 @@
       <c r="D29" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="45"/>
+      <c r="E29" s="41">
+        <v>311899</v>
+      </c>
+      <c r="F29" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="G29" s="54" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
@@ -1767,9 +2107,15 @@
       <c r="D30" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="47"/>
+      <c r="E30" s="42">
+        <v>22836000</v>
+      </c>
+      <c r="F30" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="G30" s="46" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
@@ -1778,9 +2124,15 @@
       <c r="D31" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="49"/>
+      <c r="E31" s="43">
+        <v>2330697</v>
+      </c>
+      <c r="F31" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="G31" s="48" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
@@ -1795,9 +2147,15 @@
       <c r="D32" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="40"/>
+      <c r="E32" s="39">
+        <v>2513696</v>
+      </c>
+      <c r="F32" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="G32" s="54" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
@@ -1806,9 +2164,15 @@
       <c r="D33" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="42"/>
+      <c r="E33" s="40">
+        <v>20987780</v>
+      </c>
+      <c r="F33" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="G33" s="51" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12"/>
@@ -1817,9 +2181,15 @@
       <c r="D34" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="43"/>
+      <c r="E34" s="2">
+        <v>8695176</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G34" s="59" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
@@ -1832,9 +2202,15 @@
       <c r="D35" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="45"/>
+      <c r="E35" s="41">
+        <v>5330383</v>
+      </c>
+      <c r="F35" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="G35" s="47" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
@@ -1843,9 +2219,15 @@
       <c r="D36" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="47"/>
+      <c r="E36" s="42">
+        <v>39551657</v>
+      </c>
+      <c r="F36" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="G36" s="51" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17"/>
@@ -1854,9 +2236,15 @@
       <c r="D37" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="E37" s="48"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="49"/>
+      <c r="E37" s="43">
+        <v>36010497</v>
+      </c>
+      <c r="F37" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="G37" s="52" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
@@ -1869,9 +2257,15 @@
       <c r="D38" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="50"/>
+      <c r="E38" s="3">
+        <v>8683706</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G38" s="55" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
@@ -1880,9 +2274,15 @@
       <c r="D39" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="42"/>
+      <c r="E39" s="40">
+        <v>14932242</v>
+      </c>
+      <c r="F39" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="G39" s="51" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
@@ -1891,9 +2291,15 @@
       <c r="D40" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="E40" s="51"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="52"/>
+      <c r="E40" s="44">
+        <v>292909</v>
+      </c>
+      <c r="F40" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="G40" s="52" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
@@ -1908,9 +2314,15 @@
       <c r="D41" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E41" s="44"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="45"/>
+      <c r="E41" s="41">
+        <v>25336</v>
+      </c>
+      <c r="F41" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="G41" s="54" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
@@ -1919,9 +2331,15 @@
       <c r="D42" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="47"/>
+      <c r="E42" s="42">
+        <v>918635</v>
+      </c>
+      <c r="F42" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="G42" s="46" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17"/>
@@ -1930,9 +2348,15 @@
       <c r="D43" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="49"/>
+      <c r="E43" s="43">
+        <v>1007613</v>
+      </c>
+      <c r="F43" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="G43" s="52" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
@@ -1945,9 +2369,15 @@
       <c r="D44" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="50"/>
+      <c r="E44" s="3">
+        <v>2888063</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G44" s="55" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
@@ -1956,9 +2386,15 @@
       <c r="D45" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="E45" s="41"/>
-      <c r="F45" s="41"/>
-      <c r="G45" s="42"/>
+      <c r="E45" s="40">
+        <v>1419707</v>
+      </c>
+      <c r="F45" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="G45" s="46" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="12"/>
@@ -1967,9 +2403,15 @@
       <c r="D46" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="42"/>
+      <c r="E46" s="40">
+        <v>10615296</v>
+      </c>
+      <c r="F46" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="G46" s="51" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14">
@@ -1982,9 +2424,15 @@
       <c r="D47" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E47" s="44"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="45"/>
+      <c r="E47" s="41">
+        <v>602790</v>
+      </c>
+      <c r="F47" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="G47" s="54" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
@@ -1993,9 +2441,15 @@
       <c r="D48" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E48" s="46"/>
-      <c r="F48" s="46"/>
-      <c r="G48" s="47"/>
+      <c r="E48" s="42">
+        <v>679680</v>
+      </c>
+      <c r="F48" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="G48" s="51" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="17"/>
@@ -2004,9 +2458,15 @@
       <c r="D49" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="49"/>
+      <c r="E49" s="43">
+        <v>2097334</v>
+      </c>
+      <c r="F49" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="G49" s="48" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
@@ -2019,9 +2479,15 @@
       <c r="D50" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="E50" s="41"/>
-      <c r="F50" s="41"/>
-      <c r="G50" s="42"/>
+      <c r="E50" s="40">
+        <v>1104574</v>
+      </c>
+      <c r="F50" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="G50" s="46" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
@@ -2030,9 +2496,15 @@
       <c r="D51" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="42"/>
+      <c r="E51" s="40">
+        <v>25237</v>
+      </c>
+      <c r="F51" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="G51" s="51" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="12"/>
@@ -2041,9 +2513,15 @@
       <c r="D52" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="E52" s="41"/>
-      <c r="F52" s="41"/>
-      <c r="G52" s="42"/>
+      <c r="E52" s="40">
+        <v>27085061</v>
+      </c>
+      <c r="F52" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="G52" s="46" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14">
@@ -2056,9 +2534,15 @@
       <c r="D53" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E53" s="44"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="45"/>
+      <c r="E53" s="41">
+        <v>24780</v>
+      </c>
+      <c r="F53" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="G53" s="47" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
@@ -2067,9 +2551,15 @@
       <c r="D54" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E54" s="46"/>
-      <c r="F54" s="46"/>
-      <c r="G54" s="47"/>
+      <c r="E54" s="42">
+        <v>1253213</v>
+      </c>
+      <c r="F54" s="42" t="s">
+        <v>163</v>
+      </c>
+      <c r="G54" s="46" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="17"/>
@@ -2078,9 +2568,15 @@
       <c r="D55" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E55" s="48"/>
-      <c r="F55" s="48"/>
-      <c r="G55" s="49"/>
+      <c r="E55" s="43">
+        <v>6575179</v>
+      </c>
+      <c r="F55" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="G55" s="48" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
@@ -2093,9 +2589,15 @@
       <c r="D56" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="E56" s="41"/>
-      <c r="F56" s="41"/>
-      <c r="G56" s="42"/>
+      <c r="E56" s="40">
+        <v>3822124</v>
+      </c>
+      <c r="F56" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="G56" s="51" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
@@ -2104,9 +2606,15 @@
       <c r="D57" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="E57" s="41"/>
-      <c r="F57" s="41"/>
-      <c r="G57" s="42"/>
+      <c r="E57" s="40">
+        <v>458647</v>
+      </c>
+      <c r="F57" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="G57" s="46" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="12"/>
@@ -2115,9 +2623,15 @@
       <c r="D58" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="E58" s="41"/>
-      <c r="F58" s="41"/>
-      <c r="G58" s="42"/>
+      <c r="E58" s="40">
+        <v>40675309</v>
+      </c>
+      <c r="F58" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="G58" s="46" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="14">
@@ -2130,9 +2644,15 @@
       <c r="D59" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E59" s="44"/>
-      <c r="F59" s="44"/>
-      <c r="G59" s="45"/>
+      <c r="E59" s="41">
+        <v>61542</v>
+      </c>
+      <c r="F59" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="G59" s="54" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
@@ -2141,9 +2661,15 @@
       <c r="D60" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E60" s="46"/>
-      <c r="F60" s="46"/>
-      <c r="G60" s="47"/>
+      <c r="E60" s="42">
+        <v>43149</v>
+      </c>
+      <c r="F60" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="G60" s="46" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="17"/>
@@ -2152,9 +2678,15 @@
       <c r="D61" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E61" s="48"/>
-      <c r="F61" s="48"/>
-      <c r="G61" s="49"/>
+      <c r="E61" s="43">
+        <v>37846574</v>
+      </c>
+      <c r="F61" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="G61" s="48" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
@@ -2169,9 +2701,15 @@
       <c r="D62" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="E62" s="39"/>
-      <c r="F62" s="39"/>
-      <c r="G62" s="40"/>
+      <c r="E62" s="39">
+        <v>18992270</v>
+      </c>
+      <c r="F62" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="G62" s="47" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
@@ -2180,9 +2718,15 @@
       <c r="D63" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="E63" s="41"/>
-      <c r="F63" s="41"/>
-      <c r="G63" s="42"/>
+      <c r="E63" s="40">
+        <v>20336922</v>
+      </c>
+      <c r="F63" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="G63" s="46" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12"/>
@@ -2191,9 +2735,15 @@
       <c r="D64" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="E64" s="41"/>
-      <c r="F64" s="41"/>
-      <c r="G64" s="42"/>
+      <c r="E64" s="40">
+        <v>145422</v>
+      </c>
+      <c r="F64" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="G64" s="51" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="14">
@@ -2206,9 +2756,15 @@
       <c r="D65" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E65" s="44"/>
-      <c r="F65" s="44"/>
-      <c r="G65" s="45"/>
+      <c r="E65" s="41">
+        <v>3147682</v>
+      </c>
+      <c r="F65" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="G65" s="54" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
@@ -2217,9 +2773,15 @@
       <c r="D66" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E66" s="46"/>
-      <c r="F66" s="46"/>
-      <c r="G66" s="47"/>
+      <c r="E66" s="42">
+        <v>1727530</v>
+      </c>
+      <c r="F66" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="G66" s="46" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="17"/>
@@ -2228,9 +2790,15 @@
       <c r="D67" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="E67" s="48"/>
-      <c r="F67" s="48"/>
-      <c r="G67" s="49"/>
+      <c r="E67" s="43">
+        <v>3720491</v>
+      </c>
+      <c r="F67" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="G67" s="48" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="13">
@@ -2243,9 +2811,15 @@
       <c r="D68" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E68" s="41"/>
-      <c r="F68" s="41"/>
-      <c r="G68" s="42"/>
+      <c r="E68" s="40">
+        <v>40338</v>
+      </c>
+      <c r="F68" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="G68" s="51" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
@@ -2254,9 +2828,15 @@
       <c r="D69" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="E69" s="41"/>
-      <c r="F69" s="41"/>
-      <c r="G69" s="42"/>
+      <c r="E69" s="40">
+        <v>19065069</v>
+      </c>
+      <c r="F69" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="G69" s="51" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="12"/>
@@ -2265,9 +2845,15 @@
       <c r="D70" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="E70" s="41"/>
-      <c r="F70" s="41"/>
-      <c r="G70" s="42"/>
+      <c r="E70" s="40">
+        <v>17256026</v>
+      </c>
+      <c r="F70" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="G70" s="46" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="14">
@@ -2280,9 +2866,15 @@
       <c r="D71" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="E71" s="44"/>
-      <c r="F71" s="44"/>
-      <c r="G71" s="45"/>
+      <c r="E71" s="41">
+        <v>38404397</v>
+      </c>
+      <c r="F71" s="41" t="s">
+        <v>181</v>
+      </c>
+      <c r="G71" s="47" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
@@ -2291,9 +2883,15 @@
       <c r="D72" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="E72" s="46"/>
-      <c r="F72" s="46"/>
-      <c r="G72" s="47"/>
+      <c r="E72" s="42">
+        <v>1009065</v>
+      </c>
+      <c r="F72" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="G72" s="46" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="73" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="17"/>
@@ -2302,9 +2900,15 @@
       <c r="D73" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E73" s="48"/>
-      <c r="F73" s="48"/>
-      <c r="G73" s="49"/>
+      <c r="E73" s="43">
+        <v>17907185</v>
+      </c>
+      <c r="F73" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="G73" s="48" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="13">
@@ -2317,9 +2921,15 @@
       <c r="D74" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="E74" s="41"/>
-      <c r="F74" s="41"/>
-      <c r="G74" s="42"/>
+      <c r="E74" s="40">
+        <v>9390020</v>
+      </c>
+      <c r="F74" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="G74" s="46" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
@@ -2328,9 +2938,15 @@
       <c r="D75" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="E75" s="41"/>
-      <c r="F75" s="41"/>
-      <c r="G75" s="42"/>
+      <c r="E75" s="40">
+        <v>3722597</v>
+      </c>
+      <c r="F75" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="G75" s="46" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="6"/>
@@ -2339,9 +2955,15 @@
       <c r="D76" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="E76" s="51"/>
-      <c r="F76" s="51"/>
-      <c r="G76" s="52"/>
+      <c r="E76" s="44">
+        <v>1151686</v>
+      </c>
+      <c r="F76" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="G76" s="48" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="55">

</xml_diff>